<commit_message>
finalizado cambios en auditoria servidor
</commit_message>
<xml_diff>
--- a/servidor/plantillasRegistro/plantillaConfiguracionGeneral.xlsx
+++ b/servidor/plantillasRegistro/plantillaConfiguracionGeneral.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jenny\Desktop\PROYECTOS\ProyectoFulltime\FullTimeActualizado\FullTime4.0\servidor\plantillasRegistro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC37B53E-0D4B-4737-ABD5-B643C7DBC2FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE94A085-9CBA-4A03-A1E7-3D41F23B3861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{384850A9-86C8-4587-9708-E6BD7F8E3DE2}"/>
   </bookViews>
@@ -31,21 +31,29 @@
     <sheet name="TIPO_DISCAPACIDAD" sheetId="7" r:id="rId16"/>
     <sheet name="TIPO_VACUNA" sheetId="8" r:id="rId17"/>
     <sheet name="BIOMETRICOS" sheetId="17" r:id="rId18"/>
-    <sheet name="SELECTORES" sheetId="14" state="hidden" r:id="rId19"/>
+    <sheet name="GRUPO_OCUPACIONAL" sheetId="20" r:id="rId19"/>
+    <sheet name="GRADO" sheetId="21" r:id="rId20"/>
+    <sheet name="PROCESOS" sheetId="22" r:id="rId21"/>
+    <sheet name="DETALLE_TIPO_ACCION_PERSONAL" sheetId="23" r:id="rId22"/>
+    <sheet name="SELECTORES" sheetId="14" state="hidden" r:id="rId23"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">BIOMETRICOS!$B$1:$R$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">CIUDAD_FERIADOS!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">DEPARTAMENTOS!$B$1:$D$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">DETALLE_HORARIOS!$B$1:$I$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">DETALLE_TIPO_ACCION_PERSONAL!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">EMPLEADOS!$B$1:$R$1764</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">EMPLEADOS_CARGOS!$B$1:$M$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">EMPLEADOS_CONTRATOS!$B$1:$K$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">FERIADOS!$B$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">GRADO!$B$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">GRUPO_OCUPACIONAL!$B$1:$D$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">HORARIOS!$B$1:$H$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">MODALIDAD_LABORAL!$B$1:$C$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">NIVEL_DEPARTAMENTOS!$B$1:$G$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">NIVELES_TITULOS!$B$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">PROCESOS!$B$1:$D$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">SUCURSALES!$B$1:$D$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TIPO_CARGO!$B$1:$C$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">TIPO_DISCAPACIDAD!$B$1:$C$1</definedName>
@@ -73,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="693">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="722">
   <si>
     <t>Quito</t>
   </si>
@@ -2153,13 +2161,158 @@
   </si>
   <si>
     <t>ZONA_HORARIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Datos obligatorios</t>
+  </si>
+  <si>
+    <t>INFORMACIÓN GENERAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Datos opcionales</t>
+  </si>
+  <si>
+    <t>La plantilla contiene algunas celdas con una lista de datos que deberán ser selecionadas, en el caso de hacer un ingreso manual procurar que sea la misma información de la lista de opciones para evitar errores en el ingreso de la información.</t>
+  </si>
+  <si>
+    <t>No cambiar los nombres de las pestañas que contiene la plantilla.</t>
+  </si>
+  <si>
+    <t>Datos obligatorios, si posee activo el Módulo de Acciones de Personal</t>
+  </si>
+  <si>
+    <t>En cada plantilla se encuentran datos de ejemplo que pueden ser eliminados al ingresar su información.</t>
+  </si>
+  <si>
+    <t>No cambiar los nombres de las cabeceras de la plantilla.</t>
+  </si>
+  <si>
+    <t>Todas las cabeceras se encuentran validadas en letras mayúsculas.</t>
+  </si>
+  <si>
+    <t>No eliminar ninguna de las columnas de la plantilla.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Los datos como cédulas, códigos, teléfonos y fechas estan configurados en la plantilla con un formato tipo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>texto.</t>
+    </r>
+  </si>
+  <si>
+    <t>En la plantilla las cabeceras se presentan con los siguientes colores.</t>
+  </si>
+  <si>
+    <t>La columna ITEM, deberá estar correctamente enumerada; ya que de existir errores el sistema indicará en que ITEM debe corregirse la información.</t>
+  </si>
+  <si>
+    <t>No cambiar el nombre de la plantilla, puesto que el sistema válida el nombre de este documento.</t>
+  </si>
+  <si>
+    <t>PROCESOS</t>
+  </si>
+  <si>
+    <t>DETALLE TIPO DE ACCIONES DE PERSONAL</t>
+  </si>
+  <si>
+    <t>NUMERO_PARTIDA</t>
+  </si>
+  <si>
+    <t>Gerente de Proyectos</t>
+  </si>
+  <si>
+    <t>0001254592254566333</t>
+  </si>
+  <si>
+    <t>Grado 1</t>
+  </si>
+  <si>
+    <t>PROCESO_PADRE</t>
+  </si>
+  <si>
+    <t>Habilitantes de Apoyo</t>
+  </si>
+  <si>
+    <t>Educación y Apoyo</t>
+  </si>
+  <si>
+    <t>TIPO_ACCION_PERSONAL</t>
+  </si>
+  <si>
+    <t>BASE_LEGAL</t>
+  </si>
+  <si>
+    <t>INGRESO</t>
+  </si>
+  <si>
+    <t>Ingreso a la institución con cargo Gerente</t>
+  </si>
+  <si>
+    <t>Artículo de la ley…</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">
+Para evitar errores en el sistema con respecto a la configuración de procesos considerar lo siguiente:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>1. Un proceso no puede tenerse asi mismo definido como proceso padre.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+2. Un proceso A no puede ser padre de un proceso B cuando el proceso B sea padre del proceso A.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2228,8 +2381,14 @@
       <name val="Cambria"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2248,8 +2407,26 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -2307,13 +2484,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2369,6 +2583,36 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2378,7 +2622,34 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2444,6 +2715,106 @@
         <a:xfrm>
           <a:off x="1866900" y="68580"/>
           <a:ext cx="1539240" cy="513080"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>131052</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>182881</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>4526807</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF2D61E7-E365-8DF4-4A5A-CAF34B353FCD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6402312" y="6065521"/>
+          <a:ext cx="4395755" cy="807720"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>191950</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>4632960</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>70550</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagen 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50E23C06-0CEA-EBD6-49B7-193E20B54F29}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6463210" y="7612380"/>
+          <a:ext cx="4441010" cy="1007810"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2959,6 +3330,62 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing19.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>274860</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>8160</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC0719F4-A839-42A7-A918-749ADEA14301}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22860" y="22860"/>
+          <a:ext cx="252000" cy="252000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -3003,6 +3430,174 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="45720" y="22860"/>
+          <a:ext cx="252000" cy="252000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing20.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>282480</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>540</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{258D5679-40B9-42D1-A1B9-CB8E8DF51D00}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="30480" y="15240"/>
+          <a:ext cx="252000" cy="252000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing21.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>282480</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>540</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31BFA30C-A568-48FF-9EC0-E1D92BF6EAFD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="30480" y="15240"/>
+          <a:ext cx="252000" cy="252000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing22.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>282480</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>540</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68607FE4-4F76-484F-8778-E1063BFF01ED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="30480" y="15240"/>
           <a:ext cx="252000" cy="252000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3727,10 +4322,10 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="B1:C19"/>
+  <dimension ref="B1:I39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3738,159 +4333,381 @@
     <col min="1" max="1" width="11.5546875" style="2"/>
     <col min="2" max="2" width="5.33203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="46.109375" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="11.5546875" style="2"/>
+    <col min="4" max="5" width="11.5546875" style="2"/>
+    <col min="6" max="6" width="5.33203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="71.77734375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="4.77734375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="29.44140625" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="11.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-    </row>
-    <row r="2" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="19" t="s">
+    <row r="1" spans="2:9" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+    </row>
+    <row r="2" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="29" t="s">
         <v>483</v>
       </c>
-      <c r="C2" s="20"/>
-    </row>
-    <row r="3" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="30"/>
+      <c r="F2" s="32" t="s">
+        <v>694</v>
+      </c>
+      <c r="G2" s="32"/>
+    </row>
+    <row r="3" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="16">
         <v>1</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F3" s="34">
+        <v>1</v>
+      </c>
+      <c r="G3" s="36" t="s">
+        <v>704</v>
+      </c>
+      <c r="H3" s="19"/>
+      <c r="I3" s="25" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="16">
         <v>2</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>467</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F4" s="34"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="25" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="16">
         <v>3</v>
       </c>
       <c r="C5" s="17" t="s">
         <v>468</v>
       </c>
-    </row>
-    <row r="6" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F5" s="34"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="35" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="16">
         <v>4</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>469</v>
       </c>
-    </row>
-    <row r="7" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F6" s="34"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="35"/>
+    </row>
+    <row r="7" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="16">
         <v>5</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row r="8" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F7" s="16">
+        <v>2</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="16">
         <v>6</v>
       </c>
       <c r="C8" s="17" t="s">
         <v>471</v>
       </c>
-    </row>
-    <row r="9" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F8" s="34">
+        <v>3</v>
+      </c>
+      <c r="G8" s="33" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="16">
         <v>7</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>472</v>
       </c>
-    </row>
-    <row r="10" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F9" s="34"/>
+      <c r="G9" s="33"/>
+    </row>
+    <row r="10" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="16">
         <v>8</v>
       </c>
       <c r="C10" s="17" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="11" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F10" s="34">
+        <v>4</v>
+      </c>
+      <c r="G10" s="33" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="16">
         <v>9</v>
       </c>
       <c r="C11" s="17" t="s">
         <v>474</v>
       </c>
-    </row>
-    <row r="12" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F11" s="34"/>
+      <c r="G11" s="33"/>
+    </row>
+    <row r="12" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="16">
         <v>10</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="13" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F12" s="34"/>
+      <c r="G12" s="33"/>
+    </row>
+    <row r="13" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="16">
         <v>11</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="14" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F13" s="16">
+        <v>5</v>
+      </c>
+      <c r="G13" s="21" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="16">
         <v>12</v>
       </c>
       <c r="C14" s="17" t="s">
         <v>477</v>
       </c>
-    </row>
-    <row r="15" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F14" s="16">
+        <v>6</v>
+      </c>
+      <c r="G14" s="21" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="16">
         <v>13</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="16" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F15" s="16">
+        <v>7</v>
+      </c>
+      <c r="G15" s="21" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="16">
         <v>14</v>
       </c>
       <c r="C16" s="17" t="s">
         <v>479</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F16" s="34">
+        <v>8</v>
+      </c>
+      <c r="G16" s="33" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="16">
         <v>15</v>
       </c>
       <c r="C17" s="17" t="s">
         <v>480</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F17" s="34"/>
+      <c r="G17" s="33"/>
+    </row>
+    <row r="18" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="16">
         <v>16</v>
       </c>
       <c r="C18" s="17" t="s">
         <v>481</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F18" s="34">
+        <v>9</v>
+      </c>
+      <c r="G18" s="33" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="16">
         <v>17</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>482</v>
       </c>
+      <c r="F19" s="34"/>
+      <c r="G19" s="33"/>
+    </row>
+    <row r="20" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="16">
+        <v>18</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>487</v>
+      </c>
+      <c r="F20" s="34">
+        <v>10</v>
+      </c>
+      <c r="G20" s="33" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="16">
+        <v>19</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>488</v>
+      </c>
+      <c r="F21" s="34"/>
+      <c r="G21" s="33"/>
+    </row>
+    <row r="22" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="16">
+        <v>20</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>707</v>
+      </c>
+      <c r="F22" s="39">
+        <v>11</v>
+      </c>
+      <c r="G22" s="33" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="16">
+        <v>21</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>708</v>
+      </c>
+      <c r="F23" s="40"/>
+      <c r="G23" s="33"/>
+    </row>
+    <row r="24" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F24" s="40"/>
+      <c r="G24" s="33"/>
+    </row>
+    <row r="25" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F25" s="40"/>
+      <c r="G25" s="33"/>
+    </row>
+    <row r="26" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F26" s="40"/>
+      <c r="G26" s="33"/>
+    </row>
+    <row r="27" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F27" s="40"/>
+      <c r="G27" s="33"/>
+    </row>
+    <row r="28" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F28" s="40"/>
+      <c r="G28" s="33"/>
+    </row>
+    <row r="29" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F29" s="40"/>
+      <c r="G29" s="33"/>
+    </row>
+    <row r="30" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F30" s="40"/>
+      <c r="G30" s="33"/>
+    </row>
+    <row r="31" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F31" s="40"/>
+      <c r="G31" s="33"/>
+    </row>
+    <row r="32" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F32" s="40"/>
+      <c r="G32" s="33"/>
+    </row>
+    <row r="33" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F33" s="40"/>
+      <c r="G33" s="33"/>
+    </row>
+    <row r="34" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F34" s="40"/>
+      <c r="G34" s="33"/>
+    </row>
+    <row r="35" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F35" s="40"/>
+      <c r="G35" s="33"/>
+    </row>
+    <row r="36" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F36" s="40"/>
+      <c r="G36" s="33"/>
+    </row>
+    <row r="37" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F37" s="40"/>
+      <c r="G37" s="33"/>
+    </row>
+    <row r="38" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F38" s="40"/>
+      <c r="G38" s="33"/>
+    </row>
+    <row r="39" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F39" s="41"/>
+      <c r="G39" s="33"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="19">
+    <mergeCell ref="G22:G39"/>
+    <mergeCell ref="F22:F39"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="G3:G6"/>
+    <mergeCell ref="F3:F6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G10:G12"/>
+    <mergeCell ref="F10:F12"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B1:C1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="F18:F19"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C3" location="MODALIDAD_LABORAL!B1" display="MODALIDAD LABORAL" xr:uid="{89521395-5A1F-4F67-8051-727F8213DD4F}"/>
@@ -3910,6 +4727,10 @@
     <hyperlink ref="C17" location="TIPO_DISCAPACIDAD!B1" display="TIPOS DE DISCAPACIDAD" xr:uid="{892B4864-467B-47F1-9F21-B69A3E26194C}"/>
     <hyperlink ref="C18" location="TIPO_VACUNA!B1" display="TIPOS DE VACUNA" xr:uid="{7372FC48-0EE7-4EBC-915C-263CC4F98A83}"/>
     <hyperlink ref="C19" location="BIOMETRICOS!B1" display="BIOMETRICOS" xr:uid="{C7F3D14E-FB27-466A-99A9-A597FD84B045}"/>
+    <hyperlink ref="C20" location="GRUPO_OCUPACIONAL!B1" display="GRUPO OCUPACIONAL" xr:uid="{573EE6AF-DBFE-4789-AD99-615DF0C13BAD}"/>
+    <hyperlink ref="C21" location="GRADO!B1" display="GRADO" xr:uid="{E12F4850-99BE-4EDD-818D-F9BC4EE418AC}"/>
+    <hyperlink ref="C22" location="PROCESOS!B1" display="PROCESOS" xr:uid="{7BF064A9-8B2C-4F68-9C98-D9EB747C4AE1}"/>
+    <hyperlink ref="C23" location="DETALLE_TIPO_ACCION_PERSONAL!B1" display="DETALLE TIPO DE ACCIONES DE PERSONAL" xr:uid="{933DB681-E50A-44EA-80E9-350E36790BD4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3921,8 +4742,10 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.77734375" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4031,8 +4854,10 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.77734375" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4213,8 +5038,10 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.77734375" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4294,15 +5121,18 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.6640625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.77734375" style="2" customWidth="1"/>
     <col min="2" max="2" width="10.77734375" style="2" customWidth="1"/>
-    <col min="3" max="4" width="30.6640625" style="2"/>
+    <col min="3" max="3" width="33.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="30.6640625" style="2"/>
     <col min="5" max="5" width="26.77734375" style="6" customWidth="1"/>
     <col min="6" max="6" width="21.77734375" style="2" customWidth="1"/>
     <col min="7" max="7" width="27.33203125" style="2" customWidth="1"/>
@@ -4330,10 +5160,10 @@
       <c r="G1" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="22" t="s">
         <v>435</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="22" t="s">
         <v>436</v>
       </c>
     </row>
@@ -4425,15 +5255,17 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.77734375" style="2" customWidth="1"/>
     <col min="2" max="2" width="10.77734375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="30.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.109375" style="2" customWidth="1"/>
     <col min="4" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
@@ -4471,15 +5303,18 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.77734375" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.77734375" style="4" customWidth="1"/>
     <col min="2" max="2" width="10.77734375" style="4" customWidth="1"/>
-    <col min="3" max="16384" width="30.77734375" style="4"/>
+    <col min="3" max="3" width="34.44140625" style="4" customWidth="1"/>
+    <col min="4" max="16384" width="30.77734375" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -4517,15 +5352,17 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.77734375" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.77734375" style="4" customWidth="1"/>
     <col min="2" max="2" width="10.77734375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="30.77734375" style="2"/>
+    <col min="3" max="3" width="32.21875" style="2" customWidth="1"/>
     <col min="4" max="16384" width="30.77734375" style="4"/>
   </cols>
   <sheetData>
@@ -4558,8 +5395,10 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.77734375" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4647,22 +5486,22 @@
       <c r="K1" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="22" t="s">
         <v>442</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="22" t="s">
         <v>443</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="22" t="s">
         <v>444</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="22" t="s">
         <v>446</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="22" t="s">
         <v>397</v>
       </c>
       <c r="R1" s="1" t="s">
@@ -7052,6 +7891,697 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F6C734C-FC33-4BF7-A704-1D67872920D6}">
+  <dimension ref="A1:D42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="30.77734375" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.77734375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="44.109375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="40.6640625" style="6" customWidth="1"/>
+    <col min="5" max="16384" width="30.77734375" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18"/>
+      <c r="B1" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>710</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="2"/>
+    </row>
+    <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="2"/>
+    </row>
+    <row r="21" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="2"/>
+    </row>
+    <row r="22" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C22" s="2"/>
+    </row>
+    <row r="23" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="2"/>
+    </row>
+    <row r="24" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="2"/>
+    </row>
+    <row r="25" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="2"/>
+    </row>
+    <row r="26" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="2"/>
+    </row>
+    <row r="27" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="2"/>
+    </row>
+    <row r="28" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="2"/>
+    </row>
+    <row r="29" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="2"/>
+    </row>
+    <row r="30" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C30" s="2"/>
+    </row>
+    <row r="31" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C31" s="2"/>
+    </row>
+    <row r="32" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C32" s="2"/>
+    </row>
+    <row r="33" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C33" s="2"/>
+    </row>
+    <row r="34" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C34" s="2"/>
+    </row>
+    <row r="35" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C35" s="2"/>
+    </row>
+    <row r="36" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C36" s="2"/>
+    </row>
+    <row r="37" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C37" s="2"/>
+    </row>
+    <row r="38" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C38" s="2"/>
+    </row>
+    <row r="39" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C39" s="2"/>
+    </row>
+    <row r="40" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C40" s="2"/>
+    </row>
+    <row r="41" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C41" s="2"/>
+    </row>
+    <row r="42" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C42" s="2"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:D1" xr:uid="{2F6C734C-FC33-4BF7-A704-1D67872920D6}"/>
+  <dataValidations count="1">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error dato" error="Ingrese solo numeros enteros y en orden" promptTitle="Solo numeros" sqref="B2:B133" xr:uid="{37A218A5-D446-4783-B1BB-378EC6D4A2EC}">
+      <formula1>0</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68AAF6E5-B7F7-4F51-8EE6-FF13BFB6115D}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="30.77734375" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.77734375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="30.77734375" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18"/>
+      <c r="B1" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="3"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:C1" xr:uid="{68AAF6E5-B7F7-4F51-8EE6-FF13BFB6115D}"/>
+  <dataValidations count="1">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error solo numeros" error="Ingrese solo numeros enteros y en orden" promptTitle="Solo numeros" sqref="B2:B12" xr:uid="{82D6187A-06B5-4045-A8FA-6320D917E5F1}">
+      <formula1>0</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85A238EF-2EEA-4C1B-A539-13F2F92A7A20}">
+  <dimension ref="A1:C42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="30.77734375" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.77734375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="35.77734375" style="6" customWidth="1"/>
+    <col min="4" max="16384" width="30.77734375" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18"/>
+      <c r="B1" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="2"/>
+    </row>
+    <row r="11" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="2"/>
+    </row>
+    <row r="21" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="2"/>
+    </row>
+    <row r="22" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C22" s="2"/>
+    </row>
+    <row r="23" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="2"/>
+    </row>
+    <row r="24" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="2"/>
+    </row>
+    <row r="25" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="2"/>
+    </row>
+    <row r="26" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="2"/>
+    </row>
+    <row r="27" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="2"/>
+    </row>
+    <row r="28" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="2"/>
+    </row>
+    <row r="29" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="2"/>
+    </row>
+    <row r="30" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C30" s="2"/>
+    </row>
+    <row r="31" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C31" s="2"/>
+    </row>
+    <row r="32" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C32" s="2"/>
+    </row>
+    <row r="33" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C33" s="2"/>
+    </row>
+    <row r="34" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C34" s="2"/>
+    </row>
+    <row r="35" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C35" s="2"/>
+    </row>
+    <row r="36" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C36" s="2"/>
+    </row>
+    <row r="37" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C37" s="2"/>
+    </row>
+    <row r="38" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C38" s="2"/>
+    </row>
+    <row r="39" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C39" s="2"/>
+    </row>
+    <row r="40" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C40" s="2"/>
+    </row>
+    <row r="41" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C41" s="2"/>
+    </row>
+    <row r="42" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C42" s="2"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:C1" xr:uid="{85A238EF-2EEA-4C1B-A539-13F2F92A7A20}"/>
+  <dataValidations count="1">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error dato" error="Ingrese solo numeros enteros y en orden" promptTitle="Solo numeros" sqref="B2:B133" xr:uid="{F6899BCA-CA07-4F70-8F45-DA444FB39EE8}">
+      <formula1>0</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45D8E5BE-D76B-43FB-AB2B-0CD43BC4BDDF}">
+  <dimension ref="A1:D42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="30.77734375" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.77734375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="38.33203125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="34" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="30.77734375" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18"/>
+      <c r="B1" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>715</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="2"/>
+    </row>
+    <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="18" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="19" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <autoFilter ref="B1:D1" xr:uid="{45D8E5BE-D76B-43FB-AB2B-0CD43BC4BDDF}"/>
+  <dataValidations count="1">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error dato" error="Ingrese solo numeros enteros y en orden" promptTitle="Solo numeros" sqref="B2:B133" xr:uid="{802E73C8-C84A-4148-9783-FFD380492950}">
+      <formula1>0</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EDF3D2D-C062-4025-810F-6190ED16C5CB}">
+  <dimension ref="A1:E42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="30.77734375" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.77734375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="35.77734375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="59.33203125" style="27" customWidth="1"/>
+    <col min="5" max="5" width="92.109375" style="27" customWidth="1"/>
+    <col min="6" max="16384" width="30.77734375" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18"/>
+      <c r="B1" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>716</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>385</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>718</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>719</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="2"/>
+    </row>
+    <row r="11" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="2"/>
+    </row>
+    <row r="21" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="2"/>
+    </row>
+    <row r="22" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C22" s="2"/>
+    </row>
+    <row r="23" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="2"/>
+    </row>
+    <row r="24" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="2"/>
+    </row>
+    <row r="25" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="2"/>
+    </row>
+    <row r="26" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="2"/>
+    </row>
+    <row r="27" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="2"/>
+    </row>
+    <row r="28" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="2"/>
+    </row>
+    <row r="29" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="2"/>
+    </row>
+    <row r="30" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C30" s="2"/>
+    </row>
+    <row r="31" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C31" s="2"/>
+    </row>
+    <row r="32" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C32" s="2"/>
+    </row>
+    <row r="33" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C33" s="2"/>
+    </row>
+    <row r="34" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C34" s="2"/>
+    </row>
+    <row r="35" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C35" s="2"/>
+    </row>
+    <row r="36" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C36" s="2"/>
+    </row>
+    <row r="37" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C37" s="2"/>
+    </row>
+    <row r="38" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C38" s="2"/>
+    </row>
+    <row r="39" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C39" s="2"/>
+    </row>
+    <row r="40" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C40" s="2"/>
+    </row>
+    <row r="41" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C41" s="2"/>
+    </row>
+    <row r="42" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C42" s="2"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:E1" xr:uid="{1EDF3D2D-C062-4025-810F-6190ED16C5CB}"/>
+  <dataValidations count="1">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error dato" error="Ingrese solo numeros enteros y en orden" promptTitle="Solo numeros" sqref="B2:B133" xr:uid="{9A09C606-8B7E-4505-91CB-1AD4157B70AB}">
+      <formula1>0</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CD5A4F5-BE04-4803-95A0-E9AE3C6C86A1}">
   <dimension ref="A1:F348"/>
   <sheetViews>
@@ -7068,13 +8598,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="38" t="s">
         <v>377</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
     </row>
     <row r="2" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="11" t="s">
@@ -9452,61 +10982,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68AAF6E5-B7F7-4F51-8EE6-FF13BFB6115D}">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="30.77734375" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="4.77734375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="10.77734375" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="30.77734375" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18"/>
-      <c r="B1" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="3"/>
-    </row>
-  </sheetData>
-  <autoFilter ref="B1:C1" xr:uid="{68AAF6E5-B7F7-4F51-8EE6-FF13BFB6115D}"/>
-  <dataValidations count="1">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error solo numeros" error="Ingrese solo numeros enteros y en orden" promptTitle="Solo numeros" sqref="B2:B12" xr:uid="{82D6187A-06B5-4045-A8FA-6320D917E5F1}">
-      <formula1>0</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFB5FE98-D127-4F72-80ED-0818E925ABF9}">
   <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.77734375" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -9738,8 +11222,10 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.77734375" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -9813,84 +11299,32 @@
     <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="2"/>
-    </row>
-    <row r="18" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="2"/>
-    </row>
-    <row r="19" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="2"/>
-    </row>
-    <row r="20" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="2"/>
-    </row>
-    <row r="21" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="2"/>
-    </row>
-    <row r="22" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="2"/>
-    </row>
-    <row r="23" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="2"/>
-    </row>
-    <row r="24" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="2"/>
-    </row>
-    <row r="25" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="2"/>
-    </row>
-    <row r="26" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="2"/>
-    </row>
-    <row r="27" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C27" s="2"/>
-    </row>
-    <row r="28" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="2"/>
-    </row>
-    <row r="29" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C29" s="2"/>
-    </row>
-    <row r="30" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C30" s="2"/>
-    </row>
-    <row r="31" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C31" s="2"/>
-    </row>
-    <row r="32" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C32" s="2"/>
-    </row>
-    <row r="33" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C33" s="2"/>
-    </row>
-    <row r="34" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C34" s="2"/>
-    </row>
-    <row r="35" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C35" s="2"/>
-    </row>
-    <row r="36" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C36" s="2"/>
-    </row>
-    <row r="37" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C37" s="2"/>
-    </row>
-    <row r="38" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C38" s="2"/>
-    </row>
-    <row r="39" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C39" s="2"/>
-    </row>
-    <row r="40" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C40" s="2"/>
-    </row>
-    <row r="41" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C41" s="2"/>
-    </row>
-    <row r="42" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C42" s="2"/>
-    </row>
+    <row r="17" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="18" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="19" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <autoFilter ref="B1:D1" xr:uid="{20C94F44-3285-4674-993F-F074E4017640}"/>
   <dataValidations count="1">
@@ -9908,8 +11342,10 @@
   <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.77734375" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -10071,16 +11507,18 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.77734375" style="2" customWidth="1"/>
     <col min="2" max="2" width="11.5546875" style="2"/>
-    <col min="3" max="3" width="21.44140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="21.77734375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="37.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="39.88671875" style="2" customWidth="1"/>
     <col min="5" max="5" width="11.77734375" style="2" customWidth="1"/>
     <col min="6" max="6" width="30.77734375" style="2" customWidth="1"/>
     <col min="7" max="7" width="43.44140625" style="2" customWidth="1"/>
@@ -10165,8 +11603,8 @@
   <dimension ref="A1:R1764"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
@@ -10224,13 +11662,13 @@
       <c r="M1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="23" t="s">
         <v>401</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="22" t="s">
         <v>403</v>
       </c>
       <c r="Q1" s="1" t="s">
@@ -15634,18 +17072,20 @@
     <col min="4" max="5" width="30.77734375" style="6"/>
     <col min="6" max="6" width="30.77734375" style="2"/>
     <col min="7" max="9" width="30.77734375" style="6"/>
-    <col min="10" max="16384" width="30.77734375" style="2"/>
+    <col min="10" max="11" width="30.77734375" style="2"/>
+    <col min="12" max="12" width="35.77734375" style="2" customWidth="1"/>
+    <col min="15" max="16384" width="30.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18"/>
       <c r="B1" s="5" t="s">
         <v>379</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="23" t="s">
         <v>395</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="23" t="s">
         <v>380</v>
       </c>
       <c r="E1" s="5" t="s">
@@ -15672,14 +17112,8 @@
       <c r="L1" s="5" t="s">
         <v>390</v>
       </c>
-      <c r="M1" s="5" t="s">
-        <v>487</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2">
         <v>1</v>
       </c>
@@ -15712,12 +17146,6 @@
       </c>
       <c r="L2" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>489</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>490</v>
       </c>
     </row>
   </sheetData>
@@ -15748,7 +17176,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C4FB6C7-BD8F-4FE1-BE8A-828697B5179F}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
@@ -15768,19 +17196,18 @@
     <col min="10" max="10" width="30.77734375" style="2"/>
     <col min="11" max="11" width="30.77734375" style="6"/>
     <col min="12" max="12" width="30.77734375" style="10"/>
-    <col min="13" max="13" width="30.77734375" style="2"/>
-    <col min="15" max="16384" width="30.77734375" style="2"/>
+    <col min="13" max="16384" width="30.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18"/>
       <c r="B1" s="5" t="s">
         <v>379</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="23" t="s">
         <v>380</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="22" t="s">
         <v>395</v>
       </c>
       <c r="E1" s="5" t="s">
@@ -15810,8 +17237,14 @@
       <c r="M1" s="5" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N1" s="24" t="s">
+        <v>487</v>
+      </c>
+      <c r="O1" s="24" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2">
         <v>1</v>
       </c>
@@ -15847,6 +17280,12 @@
       </c>
       <c r="M2" s="2" t="s">
         <v>24</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>490</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actualizado procesos en acciones de personal
</commit_message>
<xml_diff>
--- a/servidor/plantillasRegistro/plantillaConfiguracionGeneral.xlsx
+++ b/servidor/plantillasRegistro/plantillaConfiguracionGeneral.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jenny\Desktop\PROYECTOS\ProyectoFulltime\FullTimeActualizado\FulltimeDireccionamiento\FullTime4.0\servidor\plantillasRegistro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F58BA04-6FD8-4FE6-A3B2-B74D70E13EE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E61DF7A-1794-44F0-AD15-C2D1CFFDE43C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{384850A9-86C8-4587-9708-E6BD7F8E3DE2}"/>
   </bookViews>
@@ -32,14 +32,14 @@
     <sheet name="TIPO_DISCAPACIDAD" sheetId="7" r:id="rId17"/>
     <sheet name="TIPO_VACUNA" sheetId="8" r:id="rId18"/>
     <sheet name="BIOMETRICOS" sheetId="17" r:id="rId19"/>
-    <sheet name="GRUPO_OCUPACIONAL" sheetId="20" r:id="rId20"/>
-    <sheet name="EMPLEADO_GRUPO_OCUPACIONAL" sheetId="26" r:id="rId21"/>
-    <sheet name="GRADO" sheetId="21" r:id="rId22"/>
-    <sheet name="EMPLEADO_GRADO" sheetId="27" r:id="rId23"/>
-    <sheet name="PROCESOS" sheetId="22" r:id="rId24"/>
-    <sheet name="EMPLEADO_PROCESOS" sheetId="25" r:id="rId25"/>
+    <sheet name="GRADO" sheetId="21" r:id="rId20"/>
+    <sheet name="EMPLEADO_GRADO" sheetId="27" r:id="rId21"/>
+    <sheet name="PROCESOS" sheetId="22" r:id="rId22"/>
+    <sheet name="EMPLEADO_PROCESOS" sheetId="25" r:id="rId23"/>
+    <sheet name="GRUPO_OCUPACIONAL" sheetId="20" r:id="rId24"/>
+    <sheet name="EMPLEADO_GRUPO_OCUPACIONAL" sheetId="26" r:id="rId25"/>
     <sheet name="DETALLE_TIPO_ACCION_PERSONAL" sheetId="23" r:id="rId26"/>
-    <sheet name="SELECTORES" sheetId="14" r:id="rId27"/>
+    <sheet name="SELECTORES" sheetId="14" state="hidden" r:id="rId27"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">BIOMETRICOS!$B$1:$R$2</definedName>
@@ -51,13 +51,13 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">EMPLEADOS_CARGOS!$B$1:$M$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">EMPLEADOS_CONTRATOS!$B$1:$K$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">FERIADOS!$B$1:$E$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">GRADO!$B$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">GRUPO_OCUPACIONAL!$B$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">GRADO!$B$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="23" hidden="1">GRUPO_OCUPACIONAL!$B$1:$C$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">HORARIOS!$B$1:$H$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">MODALIDAD_LABORAL!$B$1:$C$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">NIVEL_DEPARTAMENTOS!$B$1:$G$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">NIVELES_TITULOS!$B$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="23" hidden="1">PROCESOS!$B$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">PROCESOS!$B$1:$D$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">SUCURSALES!$B$1:$D$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">TIPO_CARGO!$B$1:$C$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">TIPO_DISCAPACIDAD!$B$1:$C$1</definedName>
@@ -3579,118 +3579,6 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>22860</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>274860</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>8160</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Imagen 3">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC0719F4-A839-42A7-A918-749ADEA14301}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="22860" y="22860"/>
-          <a:ext cx="252000" cy="252000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing21.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>30480</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>282480</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>540</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagen 2">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94AABE2E-539A-4853-9AA4-37815F2E2FC5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="30480" y="15240"/>
-          <a:ext cx="252000" cy="252000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing22.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
       <xdr:colOff>30480</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>15240</xdr:rowOff>
@@ -3742,7 +3630,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing21.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -3798,7 +3686,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing22.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -3854,7 +3742,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing23.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -3898,6 +3786,118 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="38100" y="22860"/>
+          <a:ext cx="252000" cy="252000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing24.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>274860</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>8160</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC0719F4-A839-42A7-A918-749ADEA14301}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22860" y="22860"/>
+          <a:ext cx="252000" cy="252000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing25.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>282480</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>540</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94AABE2E-539A-4853-9AA4-37815F2E2FC5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="30480" y="15240"/>
           <a:ext cx="252000" cy="252000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4745,7 +4745,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4801,7 +4801,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -4815,7 +4815,7 @@
         <v>2</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -4829,7 +4829,7 @@
         <v>3</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>483</v>
+        <v>699</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -4843,7 +4843,7 @@
         <v>4</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>711</v>
+        <v>716</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -4857,7 +4857,7 @@
         <v>5</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>699</v>
+        <v>482</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -4871,7 +4871,7 @@
         <v>6</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>716</v>
+        <v>710</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -4986,14 +4986,14 @@
     <hyperlink ref="C17" location="TIPO_DISCAPACIDAD!B1" display="TIPOS DE DISCAPACIDAD" xr:uid="{892B4864-467B-47F1-9F21-B69A3E26194C}"/>
     <hyperlink ref="C18" location="TIPO_VACUNA!B1" display="TIPOS DE VACUNA" xr:uid="{7372FC48-0EE7-4EBC-915C-263CC4F98A83}"/>
     <hyperlink ref="C19" location="BIOMETRICOS!B1" display="BIOMETRICOS" xr:uid="{C7F3D14E-FB27-466A-99A9-A597FD84B045}"/>
-    <hyperlink ref="F4" location="GRUPO_OCUPACIONAL!B1" display="GRUPO OCUPACIONAL" xr:uid="{546FAC05-B651-4251-B188-B8F77026CBAA}"/>
-    <hyperlink ref="F6" location="GRADO!B1" display="GRADO" xr:uid="{A315B3C1-93A5-4C8B-9499-A80FFD2E3773}"/>
-    <hyperlink ref="F8" location="PROCESOS!B1" display="PROCESOS" xr:uid="{B623C394-7ECB-4292-8CD4-2D4AD831F513}"/>
+    <hyperlink ref="F4" location="GRADO!B1" display="GRADO" xr:uid="{A315B3C1-93A5-4C8B-9499-A80FFD2E3773}"/>
+    <hyperlink ref="F6" location="PROCESOS!B1" display="PROCESOS" xr:uid="{B623C394-7ECB-4292-8CD4-2D4AD831F513}"/>
     <hyperlink ref="F10" location="DETALLE_TIPO_ACCION_PERSONAL!B1" display="DETALLE TIPO DE ACCIONES DE PERSONAL" xr:uid="{24FAFDF3-392D-41CD-863C-3EA4D024FFD1}"/>
-    <hyperlink ref="F5" location="EMPLEADO_GRUPO_OCUPACIONAL!B1" display="EMPLEADOS GRUPO OCUPACIONAL" xr:uid="{291DB429-C1D8-4625-8D06-6008896E99C9}"/>
-    <hyperlink ref="F7" location="EMPLEADO_GRADO!B1" display="EMPLEADOS GRADO" xr:uid="{8486BD71-EE1D-48D5-AB17-59D22D70D76B}"/>
-    <hyperlink ref="F9" location="EMPLEADO_PROCESOS!A1" display="EMPLEADO PROCESOS" xr:uid="{7759AD17-F86D-4D39-A56F-B1E685540524}"/>
+    <hyperlink ref="F5" location="EMPLEADO_GRADO!B1" display="EMPLEADOS GRADO" xr:uid="{8486BD71-EE1D-48D5-AB17-59D22D70D76B}"/>
+    <hyperlink ref="F7" location="EMPLEADO_PROCESOS!A1" display="EMPLEADO PROCESOS" xr:uid="{7759AD17-F86D-4D39-A56F-B1E685540524}"/>
     <hyperlink ref="A2" location="INFORMACION_GENERAL!A1" display="INFORMACION_GENERAL!A1" xr:uid="{8E70C132-E873-4BC0-9371-A90F6E107C28}"/>
+    <hyperlink ref="F8" location="GRUPO_OCUPACIONAL!B1" display="GRUPO OCUPACIONAL" xr:uid="{E6F08FD0-F6F4-431A-81FF-A960A8374D01}"/>
+    <hyperlink ref="F9" location="EMPLEADO_GRUPO_OCUPACIONAL!B1" display="EMPLEADOS GRUPO OCUPACIONAL" xr:uid="{3E6C0140-3DCE-439F-92D6-00093E1263B9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8561,358 +8561,6 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F6C734C-FC33-4BF7-A704-1D67872920D6}">
-  <sheetPr codeName="Hoja20"/>
-  <dimension ref="A1:C42"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="30.77734375" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="4.77734375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="10.77734375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="44.109375" style="6" customWidth="1"/>
-    <col min="4" max="16384" width="30.77734375" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18"/>
-      <c r="B1" s="5" t="s">
-        <v>375</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="18"/>
-      <c r="B2" s="2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>701</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="2"/>
-    </row>
-    <row r="11" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="2"/>
-    </row>
-    <row r="12" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="2"/>
-    </row>
-    <row r="13" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="2"/>
-    </row>
-    <row r="15" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="2"/>
-    </row>
-    <row r="16" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="2"/>
-    </row>
-    <row r="17" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="2"/>
-    </row>
-    <row r="18" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="2"/>
-    </row>
-    <row r="19" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="2"/>
-    </row>
-    <row r="20" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="2"/>
-    </row>
-    <row r="21" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="2"/>
-    </row>
-    <row r="22" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="2"/>
-    </row>
-    <row r="23" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="2"/>
-    </row>
-    <row r="24" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="2"/>
-    </row>
-    <row r="25" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="2"/>
-    </row>
-    <row r="26" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="2"/>
-    </row>
-    <row r="27" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C27" s="2"/>
-    </row>
-    <row r="28" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="2"/>
-    </row>
-    <row r="29" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C29" s="2"/>
-    </row>
-    <row r="30" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C30" s="2"/>
-    </row>
-    <row r="31" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C31" s="2"/>
-    </row>
-    <row r="32" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C32" s="2"/>
-    </row>
-    <row r="33" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C33" s="2"/>
-    </row>
-    <row r="34" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C34" s="2"/>
-    </row>
-    <row r="35" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C35" s="2"/>
-    </row>
-    <row r="36" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C36" s="2"/>
-    </row>
-    <row r="37" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C37" s="2"/>
-    </row>
-    <row r="38" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C38" s="2"/>
-    </row>
-    <row r="39" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C39" s="2"/>
-    </row>
-    <row r="40" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C40" s="2"/>
-    </row>
-    <row r="41" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C41" s="2"/>
-    </row>
-    <row r="42" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C42" s="2"/>
-    </row>
-  </sheetData>
-  <autoFilter ref="B1:C1" xr:uid="{2F6C734C-FC33-4BF7-A704-1D67872920D6}"/>
-  <dataValidations count="1">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error dato" error="Ingrese solo numeros enteros y en orden" promptTitle="Solo numeros" sqref="B2:B133" xr:uid="{37A218A5-D446-4783-B1BB-378EC6D4A2EC}">
-      <formula1>0</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABE26CA4-8114-4238-A567-9909A31D1437}">
-  <sheetPr codeName="Hoja21"/>
-  <dimension ref="A1:F42"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="30.77734375" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="4.77734375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="10.77734375" style="2" customWidth="1"/>
-    <col min="3" max="5" width="32.77734375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="44.109375" style="6" customWidth="1"/>
-    <col min="7" max="16384" width="30.77734375" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18"/>
-      <c r="B1" s="5" t="s">
-        <v>375</v>
-      </c>
-      <c r="C1" s="22" t="s">
-        <v>376</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>390</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>724</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="18"/>
-      <c r="B2" s="2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>449</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>450</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>713</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>701</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F9" s="2"/>
-    </row>
-    <row r="11" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F24" s="2"/>
-    </row>
-    <row r="25" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="2"/>
-    </row>
-    <row r="26" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F26" s="2"/>
-    </row>
-    <row r="27" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F27" s="2"/>
-    </row>
-    <row r="28" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F28" s="2"/>
-    </row>
-    <row r="29" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F29" s="2"/>
-    </row>
-    <row r="30" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F30" s="2"/>
-    </row>
-    <row r="31" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F31" s="2"/>
-    </row>
-    <row r="32" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F32" s="2"/>
-    </row>
-    <row r="33" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F33" s="2"/>
-    </row>
-    <row r="34" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F34" s="2"/>
-    </row>
-    <row r="35" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F35" s="2"/>
-    </row>
-    <row r="36" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F36" s="2"/>
-    </row>
-    <row r="37" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F37" s="2"/>
-    </row>
-    <row r="38" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F38" s="2"/>
-    </row>
-    <row r="39" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F39" s="2"/>
-    </row>
-    <row r="40" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F40" s="2"/>
-    </row>
-    <row r="41" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F41" s="2"/>
-    </row>
-    <row r="42" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F42" s="2"/>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error dato" error="Ingrese solo numeros enteros y en orden" promptTitle="Solo numeros" sqref="B2:B133 E3:E133" xr:uid="{A1854DCE-9E97-4F21-B407-99743D3F67B2}">
-      <formula1>0</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85A238EF-2EEA-4C1B-A539-13F2F92A7A20}">
   <sheetPr codeName="Hoja22"/>
   <dimension ref="A1:C42"/>
@@ -9079,7 +8727,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86C1BA63-3C5F-4B14-91DD-4A80E5A8A797}">
   <sheetPr codeName="Hoja23"/>
   <dimension ref="A1:F42"/>
@@ -9264,7 +8912,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45D8E5BE-D76B-43FB-AB2B-0CD43BC4BDDF}">
   <sheetPr codeName="Hoja24"/>
   <dimension ref="A1:D42"/>
@@ -9391,7 +9039,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{727E6027-1AE6-439A-86ED-BBD888359C7C}">
   <sheetPr codeName="Hoja25"/>
   <dimension ref="A1:F42"/>
@@ -9568,6 +9216,359 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error dato" error="Ingrese solo numeros enteros y en orden" promptTitle="Solo numeros" sqref="B2:B133 E3:E133" xr:uid="{81D17666-2DD8-41CC-871E-AD2BAFC804B7}">
+      <formula1>0</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F6C734C-FC33-4BF7-A704-1D67872920D6}">
+  <sheetPr codeName="Hoja20"/>
+  <dimension ref="A1:C42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="30.77734375" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.77734375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="44.109375" style="6" customWidth="1"/>
+    <col min="4" max="16384" width="30.77734375" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18"/>
+      <c r="B1" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="18"/>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="2"/>
+    </row>
+    <row r="11" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="2"/>
+    </row>
+    <row r="21" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="2"/>
+    </row>
+    <row r="22" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C22" s="2"/>
+    </row>
+    <row r="23" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="2"/>
+    </row>
+    <row r="24" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="2"/>
+    </row>
+    <row r="25" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="2"/>
+    </row>
+    <row r="26" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="2"/>
+    </row>
+    <row r="27" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="2"/>
+    </row>
+    <row r="28" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="2"/>
+    </row>
+    <row r="29" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="2"/>
+    </row>
+    <row r="30" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C30" s="2"/>
+    </row>
+    <row r="31" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C31" s="2"/>
+    </row>
+    <row r="32" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C32" s="2"/>
+    </row>
+    <row r="33" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C33" s="2"/>
+    </row>
+    <row r="34" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C34" s="2"/>
+    </row>
+    <row r="35" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C35" s="2"/>
+    </row>
+    <row r="36" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C36" s="2"/>
+    </row>
+    <row r="37" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C37" s="2"/>
+    </row>
+    <row r="38" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C38" s="2"/>
+    </row>
+    <row r="39" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C39" s="2"/>
+    </row>
+    <row r="40" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C40" s="2"/>
+    </row>
+    <row r="41" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C41" s="2"/>
+    </row>
+    <row r="42" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C42" s="2"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:C1" xr:uid="{2F6C734C-FC33-4BF7-A704-1D67872920D6}"/>
+  <dataValidations count="1">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error dato" error="Ingrese solo numeros enteros y en orden" promptTitle="Solo numeros" sqref="B2:B133" xr:uid="{37A218A5-D446-4783-B1BB-378EC6D4A2EC}">
+      <formula1>0</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABE26CA4-8114-4238-A567-9909A31D1437}">
+  <sheetPr codeName="Hoja21"/>
+  <dimension ref="A1:F42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="B1" sqref="B1"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="30.77734375" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.77734375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" style="2" customWidth="1"/>
+    <col min="3" max="5" width="32.77734375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="44.109375" style="6" customWidth="1"/>
+    <col min="7" max="16384" width="30.77734375" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18"/>
+      <c r="B1" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>376</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>390</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>724</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="18"/>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>713</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F9" s="2"/>
+    </row>
+    <row r="11" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F32" s="2"/>
+    </row>
+    <row r="33" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F33" s="2"/>
+    </row>
+    <row r="34" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F34" s="2"/>
+    </row>
+    <row r="35" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F35" s="2"/>
+    </row>
+    <row r="36" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F36" s="2"/>
+    </row>
+    <row r="37" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F37" s="2"/>
+    </row>
+    <row r="38" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F38" s="2"/>
+    </row>
+    <row r="39" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F39" s="2"/>
+    </row>
+    <row r="40" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F40" s="2"/>
+    </row>
+    <row r="41" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F41" s="2"/>
+    </row>
+    <row r="42" spans="6:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F42" s="2"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error dato" error="Ingrese solo numeros enteros y en orden" promptTitle="Solo numeros" sqref="B2:B133 E3:E133" xr:uid="{A1854DCE-9E97-4F21-B407-99743D3F67B2}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -9763,7 +9764,7 @@
   <dimension ref="A1:G348"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.77734375" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
actualizado todas las ramas
</commit_message>
<xml_diff>
--- a/servidor/plantillasRegistro/plantillaConfiguracionGeneral.xlsx
+++ b/servidor/plantillasRegistro/plantillaConfiguracionGeneral.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jenny\Desktop\PROYECTOS\ProyectoFulltime\FullTimeActualizado\FulltimeDireccionamiento\FullTime4.0\servidor\plantillasRegistro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E61DF7A-1794-44F0-AD15-C2D1CFFDE43C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5EFB78-B251-4B9B-B984-CA8C32CCDD89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{384850A9-86C8-4587-9708-E6BD7F8E3DE2}"/>
   </bookViews>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="730">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="729">
   <si>
     <t>Quito</t>
   </si>
@@ -146,9 +146,6 @@
   </si>
   <si>
     <t>Pichincha</t>
-  </si>
-  <si>
-    <t>Soltero/a</t>
   </si>
   <si>
     <t>Femenino</t>
@@ -4745,7 +4742,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4770,11 +4767,11 @@
         <v>#VALUE!</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C2" s="34"/>
       <c r="E2" s="30" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="F2" s="31"/>
     </row>
@@ -4783,10 +4780,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="E3" s="32" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="F3" s="32"/>
     </row>
@@ -4795,13 +4792,13 @@
         <v>2</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E4" s="16">
         <v>1</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -4809,13 +4806,13 @@
         <v>3</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="E5" s="16">
         <v>2</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -4823,13 +4820,13 @@
         <v>4</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="E6" s="16">
         <v>3</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -4837,13 +4834,13 @@
         <v>5</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="E7" s="16">
         <v>4</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -4851,13 +4848,13 @@
         <v>6</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E8" s="16">
         <v>5</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -4865,13 +4862,13 @@
         <v>7</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E9" s="16">
         <v>6</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -4879,13 +4876,13 @@
         <v>8</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E10" s="16">
         <v>7</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -4893,7 +4890,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -4901,7 +4898,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -4909,7 +4906,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -4917,7 +4914,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -4925,7 +4922,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -4933,7 +4930,7 @@
         <v>14</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -4941,7 +4938,7 @@
         <v>15</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="18" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -4949,7 +4946,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -4957,7 +4954,7 @@
         <v>17</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
   </sheetData>
@@ -5029,40 +5026,40 @@
     <row r="1" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18"/>
       <c r="B1" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="C1" s="22" t="s">
         <v>375</v>
       </c>
-      <c r="C1" s="22" t="s">
-        <v>376</v>
-      </c>
       <c r="D1" s="21" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>403</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>407</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>403</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>404</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>387</v>
-      </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="13" t="s">
         <v>408</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="M1" s="5" t="s">
         <v>409</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -5071,37 +5068,37 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>450</v>
-      </c>
       <c r="E2" s="6" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>11</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L2" s="10">
         <v>150</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -5152,16 +5149,16 @@
     <row r="1" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18"/>
       <c r="B1" s="5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="5" t="s">
         <v>381</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -5170,10 +5167,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -5181,13 +5178,13 @@
         <v>2</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>484</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>485</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="6" t="s">
         <v>486</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -5265,16 +5262,16 @@
     <row r="1" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18"/>
       <c r="B1" s="5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>384</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -5289,7 +5286,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -5451,25 +5448,25 @@
     <row r="1" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18"/>
       <c r="B1" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>424</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>429</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>426</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -5478,22 +5475,22 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F2" s="2">
         <v>30</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
   </sheetData>
@@ -5540,28 +5537,28 @@
     <row r="1" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18"/>
       <c r="B1" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H1" s="21" t="s">
+        <v>429</v>
+      </c>
+      <c r="I1" s="21" t="s">
         <v>430</v>
-      </c>
-      <c r="I1" s="21" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -5570,13 +5567,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F2" s="15">
         <v>0</v>
@@ -5587,13 +5584,13 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="F3" s="15"/>
     </row>
@@ -5602,13 +5599,13 @@
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F4" s="15"/>
     </row>
@@ -5617,17 +5614,17 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F5" s="15"/>
       <c r="G5" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
   </sheetData>
@@ -5671,10 +5668,10 @@
     <row r="1" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18"/>
       <c r="B1" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -5721,13 +5718,13 @@
     <row r="1" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18"/>
       <c r="B1" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>376</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -5772,10 +5769,10 @@
     <row r="1" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18"/>
       <c r="B1" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -5816,10 +5813,10 @@
     <row r="1" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18"/>
       <c r="B1" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -5864,55 +5861,55 @@
     <row r="1" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18"/>
       <c r="B1" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>432</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
+        <v>388</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>389</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>457</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>460</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="21" t="s">
         <v>436</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="M1" s="21" t="s">
         <v>437</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="N1" s="21" t="s">
         <v>438</v>
       </c>
-      <c r="N1" s="21" t="s">
+      <c r="O1" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="21" t="s">
         <v>440</v>
       </c>
-      <c r="P1" s="21" t="s">
-        <v>441</v>
-      </c>
       <c r="Q1" s="21" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="2" spans="1:19" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -5927,34 +5924,34 @@
         <v>2</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>446</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>447</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>448</v>
       </c>
       <c r="H2" s="2">
         <v>4370</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>458</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>411</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>459</v>
-      </c>
       <c r="L2" s="2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="O2" s="2">
         <v>12345</v>
@@ -5962,7 +5959,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="S2" s="4"/>
     </row>
@@ -8325,7 +8322,7 @@
     </row>
     <row r="2" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="36" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="C2" s="36"/>
       <c r="D2" s="36"/>
@@ -8336,11 +8333,11 @@
         <v>1</v>
       </c>
       <c r="C3" s="41" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="23" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -8348,7 +8345,7 @@
       <c r="C4" s="42"/>
       <c r="D4" s="20"/>
       <c r="E4" s="23" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -8356,7 +8353,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="37" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D5" s="37"/>
       <c r="E5" s="37"/>
@@ -8366,7 +8363,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="43" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="D6" s="43"/>
       <c r="E6" s="43"/>
@@ -8376,7 +8373,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="43" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="D7" s="43"/>
       <c r="E7" s="43"/>
@@ -8392,7 +8389,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="D9" s="37"/>
       <c r="E9" s="37"/>
@@ -8402,7 +8399,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="37" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="D10" s="37"/>
       <c r="E10" s="37"/>
@@ -8412,7 +8409,7 @@
         <v>7</v>
       </c>
       <c r="C11" s="37" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="D11" s="37"/>
       <c r="E11" s="37"/>
@@ -8422,7 +8419,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="43" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D12" s="43"/>
       <c r="E12" s="43"/>
@@ -8432,7 +8429,7 @@
         <v>9</v>
       </c>
       <c r="C13" s="43" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="D13" s="43"/>
       <c r="E13" s="43"/>
@@ -8448,7 +8445,7 @@
         <v>10</v>
       </c>
       <c r="C15" s="43" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="D15" s="43"/>
       <c r="E15" s="43"/>
@@ -8458,7 +8455,7 @@
         <v>11</v>
       </c>
       <c r="C16" s="43" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="D16" s="43"/>
       <c r="E16" s="43"/>
@@ -8583,10 +8580,10 @@
     <row r="1" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18"/>
       <c r="B1" s="5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -8595,7 +8592,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -8751,19 +8748,19 @@
     <row r="1" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18"/>
       <c r="B1" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="C1" s="22" t="s">
         <v>375</v>
       </c>
-      <c r="C1" s="22" t="s">
-        <v>376</v>
-      </c>
       <c r="D1" s="22" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -8772,16 +8769,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>450</v>
-      </c>
       <c r="E2" s="6" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -8936,13 +8933,13 @@
     <row r="1" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18"/>
       <c r="B1" s="5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -8951,7 +8948,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -8959,10 +8956,10 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -9048,7 +9045,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.77734375" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -9063,19 +9060,19 @@
     <row r="1" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18"/>
       <c r="B1" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="C1" s="22" t="s">
         <v>375</v>
       </c>
-      <c r="C1" s="22" t="s">
-        <v>376</v>
-      </c>
       <c r="D1" s="22" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -9084,16 +9081,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>450</v>
-      </c>
       <c r="E2" s="6" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -9247,10 +9244,10 @@
     <row r="1" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18"/>
       <c r="B1" s="5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -9259,7 +9256,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -9416,19 +9413,19 @@
     <row r="1" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18"/>
       <c r="B1" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="C1" s="22" t="s">
         <v>375</v>
       </c>
-      <c r="C1" s="22" t="s">
-        <v>376</v>
-      </c>
       <c r="D1" s="22" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -9437,16 +9434,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>450</v>
-      </c>
       <c r="E2" s="6" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -9602,16 +9599,16 @@
     <row r="1" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18"/>
       <c r="B1" s="5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>704</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>380</v>
+      </c>
+      <c r="E1" s="26" t="s">
         <v>705</v>
-      </c>
-      <c r="D1" s="24" t="s">
-        <v>381</v>
-      </c>
-      <c r="E1" s="26" t="s">
-        <v>706</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -9620,13 +9617,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>706</v>
+      </c>
+      <c r="D2" s="25" t="s">
         <v>707</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="E2" s="25" t="s">
         <v>708</v>
-      </c>
-      <c r="E2" s="25" t="s">
-        <v>709</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -9764,7 +9761,7 @@
   <dimension ref="A1:G348"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.77734375" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -9778,7 +9775,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="44" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C1" s="44"/>
       <c r="D1" s="44"/>
@@ -9787,22 +9784,22 @@
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="D2" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="11" t="s">
-        <v>29</v>
-      </c>
       <c r="E2" s="11" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -9810,22 +9807,22 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -9833,22 +9830,22 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -9856,13 +9853,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -9870,13 +9867,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -9884,2282 +9881,2282 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D8" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D9" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D10" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D11" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D12" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D13" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D14" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D15" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D16" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="17" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D17" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="18" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D18" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="19" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D19" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="20" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D20" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="21" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D21" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="22" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D22" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="23" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D23" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="24" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D24" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="25" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D25" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="26" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D26" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="27" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D27" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="28" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D28" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="29" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D29" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="30" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D30" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="31" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D31" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="32" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D32" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="33" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D33" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="34" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D34" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="35" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D35" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="36" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D36" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="37" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D37" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="38" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D38" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="39" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D39" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="40" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D40" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="41" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D41" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="42" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D42" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="43" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D43" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="44" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D44" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="45" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D45" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="46" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D46" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="47" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D47" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="48" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D48" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="49" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D49" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="50" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D50" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="51" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D51" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="52" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D52" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="53" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D53" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="54" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D54" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="55" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D55" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="56" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D56" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="57" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D57" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="58" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D58" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="59" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D59" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="60" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D60" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="61" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D61" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="62" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D62" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="63" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D63" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="64" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D64" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="65" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D65" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="66" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D66" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="67" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D67" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="68" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D68" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="69" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D69" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="70" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D70" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="71" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D71" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="72" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D72" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="73" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D73" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="74" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D74" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="75" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D75" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="76" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D76" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="77" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D77" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="78" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D78" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="79" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D79" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="80" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D80" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="81" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D81" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="82" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D82" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="83" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D83" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="84" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D84" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="85" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D85" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="86" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D86" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="87" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D87" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="88" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D88" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F88" s="4" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="89" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D89" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="90" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D90" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F90" s="4" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="91" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D91" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F91" s="4" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="92" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D92" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F92" s="4" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="93" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D93" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F93" s="4" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="94" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D94" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F94" s="4" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="95" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D95" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F95" s="4" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="96" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D96" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F96" s="4" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="97" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D97" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F97" s="4" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="98" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D98" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F98" s="4" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="99" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D99" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F99" s="4" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="100" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D100" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F100" s="4" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="101" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D101" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F101" s="4" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="102" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D102" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F102" s="4" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="103" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D103" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F103" s="4" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="104" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D104" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F104" s="4" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="105" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D105" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F105" s="4" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="106" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D106" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F106" s="4" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="107" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D107" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F107" s="4" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="108" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D108" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F108" s="4" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="109" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D109" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F109" s="4" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="110" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D110" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F110" s="4" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="111" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D111" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F111" s="4" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="112" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D112" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F112" s="4" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="113" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D113" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F113" s="4" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="114" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D114" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F114" s="4" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="115" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D115" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F115" s="4" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="116" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D116" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F116" s="4" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="117" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D117" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F117" s="4" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="118" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D118" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F118" s="4" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="119" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D119" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F119" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="120" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D120" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F120" s="4" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="121" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D121" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F121" s="4" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="122" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D122" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F122" s="4" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="123" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D123" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F123" s="4" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="124" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D124" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F124" s="4" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="125" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D125" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F125" s="4" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="126" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D126" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F126" s="4" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="127" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D127" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F127" s="4" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="128" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D128" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F128" s="4" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="129" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D129" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F129" s="4" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="130" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D130" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F130" s="4" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="131" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D131" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F131" s="4" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="132" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D132" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F132" s="4" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="133" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D133" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F133" s="4" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="134" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D134" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F134" s="4" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="135" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D135" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F135" s="4" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="136" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D136" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F136" s="4" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="137" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D137" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F137" s="4" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="138" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D138" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F138" s="4" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="139" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D139" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F139" s="4" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="140" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D140" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F140" s="4" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="141" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D141" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F141" s="4" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="142" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D142" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F142" s="4" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="143" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D143" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F143" s="4" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="144" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D144" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F144" s="4" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="145" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D145" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F145" s="4" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="146" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D146" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F146" s="4" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="147" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D147" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F147" s="4" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="148" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D148" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F148" s="4" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="149" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D149" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F149" s="4" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="150" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D150" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F150" s="4" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="151" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D151" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F151" s="4" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="152" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D152" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F152" s="4" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="153" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D153" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F153" s="4" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="154" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D154" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F154" s="4" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="155" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D155" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F155" s="4" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="156" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D156" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F156" s="4" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="157" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D157" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F157" s="4" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="158" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D158" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F158" s="4" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="159" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D159" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F159" s="4" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="160" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D160" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F160" s="4" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="161" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D161" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F161" s="4" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="162" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D162" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F162" s="4" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="163" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D163" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F163" s="4" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="164" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D164" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F164" s="4" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="165" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D165" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F165" s="4" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="166" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D166" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F166" s="4" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="167" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D167" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F167" s="4" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="168" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D168" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F168" s="4" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="169" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D169" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F169" s="4" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="170" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D170" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F170" s="4" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="171" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D171" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F171" s="4" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="172" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D172" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F172" s="4" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="173" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D173" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F173" s="4" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="174" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D174" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F174" s="4" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="175" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D175" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F175" s="4" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="176" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D176" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F176" s="4" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="177" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D177" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F177" s="4" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="178" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D178" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F178" s="4" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="179" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D179" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F179" s="4" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="180" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D180" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F180" s="4" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="181" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D181" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F181" s="4" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="182" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D182" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F182" s="4" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="183" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D183" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F183" s="4" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="184" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D184" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F184" s="4" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="185" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D185" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F185" s="4" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="186" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D186" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F186" s="4" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="187" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D187" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F187" s="4" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="188" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D188" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F188" s="4" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="189" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D189" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F189" s="4" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="190" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D190" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F190" s="4" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="191" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D191" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F191" s="4" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="192" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D192" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F192" s="4" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="193" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D193" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F193" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="194" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D194" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F194" s="4" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="195" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D195" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F195" s="4" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="196" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D196" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="197" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D197" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="198" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D198" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="199" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D199" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="200" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D200" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="201" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D201" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="202" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D202" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="203" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D203" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="204" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D204" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="205" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D205" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="206" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D206" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="207" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D207" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="208" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D208" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="209" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D209" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="210" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D210" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="211" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D211" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="212" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D212" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="213" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D213" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="214" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D214" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="215" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D215" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="216" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D216" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="217" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D217" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="218" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D218" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="219" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D219" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="220" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D220" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="221" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D221" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="222" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D222" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="223" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D223" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="224" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D224" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="225" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D225" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="226" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D226" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="227" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D227" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="228" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D228" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="229" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D229" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="230" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D230" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="231" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D231" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="232" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D232" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="233" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D233" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="234" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D234" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="235" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D235" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="236" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D236" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="237" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D237" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="238" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D238" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="239" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D239" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="240" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D240" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="241" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D241" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="242" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D242" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="243" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D243" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="244" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D244" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="245" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D245" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="246" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D246" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="247" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D247" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="248" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D248" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="249" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D249" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="250" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D250" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="251" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D251" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="252" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D252" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="253" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D253" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="254" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D254" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="255" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D255" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="256" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D256" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="257" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D257" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="258" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D258" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="259" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D259" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="260" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D260" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="261" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D261" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="262" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D262" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="263" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D263" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="264" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D264" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="265" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D265" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="266" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D266" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="267" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D267" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="268" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D268" s="4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="269" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D269" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="270" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D270" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="271" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D271" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="272" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D272" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="273" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D273" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="274" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D274" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="275" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D275" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="276" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D276" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="277" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D277" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="278" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D278" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="279" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D279" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="280" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D280" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="281" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D281" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="282" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D282" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="283" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D283" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="284" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D284" s="4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="285" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D285" s="4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="286" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D286" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="287" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D287" s="4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="288" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D288" s="4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="289" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D289" s="4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="290" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D290" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="291" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D291" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="292" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D292" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="293" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D293" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="294" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D294" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="295" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D295" s="4" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="296" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D296" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="297" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D297" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="298" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D298" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="299" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D299" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="300" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D300" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="301" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D301" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="302" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D302" s="4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="303" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D303" s="4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="304" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D304" s="4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="305" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D305" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="306" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D306" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="307" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D307" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="308" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D308" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="309" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D309" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="310" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D310" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="311" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D311" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="312" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D312" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="313" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D313" s="4" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="314" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D314" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="315" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D315" s="4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="316" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D316" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="317" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D317" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="318" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D318" s="4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="319" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D319" s="4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="320" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D320" s="4" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="321" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D321" s="4" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="322" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D322" s="4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="323" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D323" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="324" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D324" s="4" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="325" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D325" s="4" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="326" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D326" s="4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="327" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D327" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="328" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D328" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="329" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D329" s="4" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="330" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D330" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="331" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D331" s="4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="332" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D332" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="333" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D333" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="334" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D334" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="335" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D335" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="336" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D336" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="337" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D337" s="4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="338" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D338" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="339" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D339" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="340" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D340" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="341" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D341" s="4" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="342" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D342" s="4" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="343" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D343" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="344" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D344" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="345" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D345" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="346" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D346" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="347" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D347" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="348" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D348" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
   </sheetData>
@@ -12193,10 +12190,10 @@
     <row r="1" spans="1:3" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18"/>
       <c r="B1" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -12205,7 +12202,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -12246,10 +12243,10 @@
     <row r="1" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18"/>
       <c r="B1" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -12484,13 +12481,13 @@
     <row r="1" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18"/>
       <c r="B1" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>376</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -12605,13 +12602,13 @@
     <row r="1" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18"/>
       <c r="B1" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>376</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -12776,22 +12773,22 @@
     <row r="1" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18"/>
       <c r="B1" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>443</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>444</v>
       </c>
       <c r="H1" s="11"/>
       <c r="I1" s="11"/>
@@ -12834,7 +12831,7 @@
         <v>2</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>1</v>
@@ -12853,10 +12850,10 @@
   <dimension ref="A1:T1764"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T2" sqref="T2"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.77734375" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -12881,61 +12878,61 @@
     <row r="1" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18"/>
       <c r="B1" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>723</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>388</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>725</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>724</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>389</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>376</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="5" t="s">
         <v>391</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="5" t="s">
         <v>394</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="O1" s="22" t="s">
         <v>395</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="O1" s="22" t="s">
+      <c r="P1" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="21" t="s">
         <v>397</v>
       </c>
-      <c r="Q1" s="21" t="s">
+      <c r="R1" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="S1" s="1" t="s">
-        <v>400</v>
-      </c>
       <c r="T1" s="21" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -12944,49 +12941,49 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E2" s="6">
         <v>1275</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>450</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>451</v>
       </c>
       <c r="I2" s="6">
         <v>12345</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>716</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="6" t="s">
         <v>452</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="L2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="O2" s="6" t="s">
+        <v>480</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q2" s="2" t="s">
         <v>453</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>481</v>
-      </c>
-      <c r="P2" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>454</v>
       </c>
       <c r="R2" s="2">
         <v>-0.29974331775556401</v>
@@ -18351,37 +18348,37 @@
     <row r="1" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18"/>
       <c r="B1" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>389</v>
+      </c>
+      <c r="D1" s="22" t="s">
         <v>375</v>
       </c>
-      <c r="C1" s="22" t="s">
-        <v>390</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>376</v>
-      </c>
       <c r="E1" s="5" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>401</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>402</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>403</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>404</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>405</v>
       </c>
-      <c r="K1" s="5" t="s">
-        <v>406</v>
-      </c>
       <c r="L1" s="5" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -18390,34 +18387,34 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>450</v>
-      </c>
       <c r="E2" s="6" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>20</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>11</v>
       </c>
       <c r="I2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actualizado informacion del timbre
</commit_message>
<xml_diff>
--- a/servidor/plantillasRegistro/plantillaConfiguracionGeneral.xlsx
+++ b/servidor/plantillasRegistro/plantillaConfiguracionGeneral.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jenny\Desktop\PROYECTOS\ProyectoFulltime\FullTimeActualizado\FulltimeDireccionamiento\FullTime4.0\servidor\plantillasRegistro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5EFB78-B251-4B9B-B984-CA8C32CCDD89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C5BE36-5EA9-4582-B8F0-53A3D01F5DF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{384850A9-86C8-4587-9708-E6BD7F8E3DE2}"/>
   </bookViews>
@@ -2668,15 +2668,6 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2693,7 +2684,16 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4742,7 +4742,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5709,10 +5709,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.77734375" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.77734375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="10.77734375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="34.44140625" style="4" customWidth="1"/>
-    <col min="4" max="16384" width="30.77734375" style="4"/>
+    <col min="1" max="1" width="4.77734375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="34.44140625" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="30.77734375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -5760,10 +5760,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.77734375" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.77734375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="10.77734375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="4.77734375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" style="2" customWidth="1"/>
     <col min="3" max="3" width="32.21875" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="30.77734375" style="4"/>
+    <col min="4" max="16384" width="30.77734375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -5805,9 +5805,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.77734375" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.77734375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="10.77734375" style="4" customWidth="1"/>
-    <col min="3" max="16384" width="30.77734375" style="4"/>
+    <col min="1" max="1" width="4.77734375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="30.77734375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -8315,24 +8315,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
     </row>
     <row r="2" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="43" t="s">
         <v>686</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
     </row>
     <row r="3" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="39">
+      <c r="B3" s="36">
         <v>1</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="38" t="s">
         <v>695</v>
       </c>
       <c r="D3" s="19"/>
@@ -8341,8 +8341,8 @@
       </c>
     </row>
     <row r="4" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="40"/>
-      <c r="C4" s="42"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="39"/>
       <c r="D4" s="20"/>
       <c r="E4" s="23" t="s">
         <v>687</v>
@@ -8352,188 +8352,193 @@
       <c r="B5" s="16">
         <v>2</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="40" t="s">
         <v>693</v>
       </c>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
     </row>
     <row r="6" spans="2:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="16">
         <v>3</v>
       </c>
-      <c r="C6" s="43" t="s">
+      <c r="C6" s="41" t="s">
         <v>694</v>
       </c>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
     </row>
     <row r="7" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="38">
+      <c r="B7" s="35">
         <v>4</v>
       </c>
-      <c r="C7" s="43" t="s">
+      <c r="C7" s="41" t="s">
         <v>688</v>
       </c>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
     </row>
     <row r="8" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="38"/>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
     </row>
     <row r="9" spans="2:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="28">
         <v>5</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="40" t="s">
         <v>689</v>
       </c>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
     </row>
     <row r="10" spans="2:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="16">
         <v>6</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="40" t="s">
         <v>691</v>
       </c>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
     </row>
     <row r="11" spans="2:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="16">
         <v>7</v>
       </c>
-      <c r="C11" s="37" t="s">
+      <c r="C11" s="40" t="s">
         <v>692</v>
       </c>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
     </row>
     <row r="12" spans="2:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="27">
         <v>8</v>
       </c>
-      <c r="C12" s="43" t="s">
+      <c r="C12" s="41" t="s">
         <v>690</v>
       </c>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
     </row>
     <row r="13" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="39">
+      <c r="B13" s="36">
         <v>9</v>
       </c>
-      <c r="C13" s="43" t="s">
+      <c r="C13" s="41" t="s">
         <v>696</v>
       </c>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
     </row>
     <row r="14" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="40"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
     </row>
     <row r="15" spans="2:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="27">
         <v>10</v>
       </c>
-      <c r="C15" s="43" t="s">
+      <c r="C15" s="41" t="s">
         <v>697</v>
       </c>
-      <c r="D15" s="43"/>
-      <c r="E15" s="43"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
     </row>
     <row r="16" spans="2:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="38">
+      <c r="B16" s="35">
         <v>11</v>
       </c>
-      <c r="C16" s="43" t="s">
+      <c r="C16" s="41" t="s">
         <v>722</v>
       </c>
-      <c r="D16" s="43"/>
-      <c r="E16" s="43"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
     </row>
     <row r="17" spans="2:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="38"/>
-      <c r="C17" s="43"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
     </row>
     <row r="18" spans="2:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="38"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="43"/>
-      <c r="E18" s="43"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
     </row>
     <row r="19" spans="2:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="38"/>
-      <c r="C19" s="43"/>
-      <c r="D19" s="43"/>
-      <c r="E19" s="43"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
     </row>
     <row r="20" spans="2:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="38"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
     </row>
     <row r="21" spans="2:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="38"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="41"/>
     </row>
     <row r="22" spans="2:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="38"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="43"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="41"/>
     </row>
     <row r="23" spans="2:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="38"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="43"/>
+      <c r="B23" s="35"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="41"/>
     </row>
     <row r="24" spans="2:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="38"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="43"/>
+      <c r="B24" s="35"/>
+      <c r="C24" s="41"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="41"/>
     </row>
     <row r="25" spans="2:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="38"/>
-      <c r="C25" s="43"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="43"/>
+      <c r="B25" s="35"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="41"/>
     </row>
     <row r="26" spans="2:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="38"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="43"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="41"/>
     </row>
     <row r="27" spans="2:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="38"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
+      <c r="B27" s="35"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="41"/>
     </row>
     <row r="28" spans="2:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="38"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
+      <c r="B28" s="35"/>
+      <c r="C28" s="41"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:E11"/>
     <mergeCell ref="B16:B28"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
@@ -8546,11 +8551,6 @@
     <mergeCell ref="C16:E28"/>
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="C13:E14"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>